<commit_message>
Updated Tableau plots and input validation in script
</commit_message>
<xml_diff>
--- a/Plotting Results/EPA_CA2_X00129654.xlsx
+++ b/Plotting Results/EPA_CA2_X00129654.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{E4126FAF-66DE-430F-A4B2-7565DBFD5007}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{034FF748-267D-468F-A35B-281A85A7EDF8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -349,7 +349,7 @@
   <dimension ref="A1:C51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -367,552 +367,552 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>10</v>
+        <v>6</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>41.52</v>
+        <v>90.48</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>21</v>
+        <v>12</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3">
-        <v>41.43</v>
+        <v>89.7</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>32</v>
+        <v>18</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4">
-        <v>41.34</v>
+        <v>92.75</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5">
-        <v>41.25</v>
+        <v>91.44</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6">
-        <v>41.15</v>
+        <v>91.69</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>65</v>
+        <v>36</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7">
-        <v>41.06</v>
+        <v>90.23</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>76</v>
+        <v>42</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8">
-        <v>40.98</v>
+        <v>91.44</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>87</v>
+        <v>48</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9">
-        <v>40.89</v>
+        <v>91.44</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>98</v>
+        <v>54</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10">
-        <v>40.799999999999997</v>
+        <v>91.25</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>109</v>
+        <v>60</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11">
-        <v>40.71</v>
+        <v>91.21</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>122</v>
+        <v>66</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12">
-        <v>40.6</v>
+        <v>91.46</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>135</v>
+        <v>72</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13">
-        <v>40.47</v>
+        <v>92.42</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>148</v>
+        <v>78</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14">
-        <v>40.35</v>
+        <v>90.48</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>161</v>
+        <v>84</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15">
-        <v>40.22</v>
+        <v>90.98</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>174</v>
+        <v>90</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
       <c r="C16">
-        <v>40.090000000000003</v>
+        <v>92.46</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>187</v>
+        <v>96</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
       <c r="C17">
-        <v>39.97</v>
+        <v>91.18</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>200</v>
+        <v>102</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
       <c r="C18">
-        <v>39.86</v>
+        <v>91.69</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>213</v>
+        <v>108</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
       <c r="C19">
-        <v>39.74</v>
+        <v>92.42</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>226</v>
+        <v>114</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
       <c r="C20">
-        <v>39.630000000000003</v>
+        <v>90.45</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>239</v>
+        <v>120</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
       <c r="C21">
-        <v>39.520000000000003</v>
+        <v>90.7</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>252</v>
+        <v>126</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
       <c r="C22">
-        <v>39.43</v>
+        <v>91.18</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>265</v>
+        <v>132</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
       <c r="C23">
-        <v>39.33</v>
+        <v>91.46</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>278</v>
+        <v>138</v>
       </c>
       <c r="B24">
         <v>23</v>
       </c>
       <c r="C24">
-        <v>39.229999999999997</v>
+        <v>90.7</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>291</v>
+        <v>144</v>
       </c>
       <c r="B25">
         <v>24</v>
       </c>
       <c r="C25">
-        <v>39.15</v>
+        <v>92.95</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>304</v>
+        <v>150</v>
       </c>
       <c r="B26">
         <v>25</v>
       </c>
       <c r="C26">
-        <v>39.049999999999997</v>
+        <v>90.5</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>317</v>
+        <v>156</v>
       </c>
       <c r="B27">
         <v>26</v>
       </c>
       <c r="C27">
-        <v>38.950000000000003</v>
+        <v>91.21</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>330</v>
+        <v>162</v>
       </c>
       <c r="B28">
         <v>27</v>
       </c>
       <c r="C28">
-        <v>38.86</v>
+        <v>91.71</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>343</v>
+        <v>168</v>
       </c>
       <c r="B29">
         <v>28</v>
       </c>
       <c r="C29">
-        <v>38.78</v>
+        <v>91.67</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>356</v>
+        <v>174</v>
       </c>
       <c r="B30">
         <v>29</v>
       </c>
       <c r="C30">
-        <v>38.69</v>
+        <v>90.25</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>369</v>
+        <v>180</v>
       </c>
       <c r="B31">
         <v>30</v>
       </c>
       <c r="C31">
-        <v>38.6</v>
+        <v>92.7</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>382</v>
+        <v>186</v>
       </c>
       <c r="B32">
         <v>31</v>
       </c>
       <c r="C32">
-        <v>38.51</v>
+        <v>91.18</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>395</v>
+        <v>192</v>
       </c>
       <c r="B33">
         <v>32</v>
       </c>
       <c r="C33">
-        <v>38.43</v>
+        <v>91.5</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>408</v>
+        <v>198</v>
       </c>
       <c r="B34">
         <v>33</v>
       </c>
       <c r="C34">
-        <v>38.340000000000003</v>
+        <v>92.96</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>421</v>
+        <v>204</v>
       </c>
       <c r="B35">
         <v>34</v>
       </c>
       <c r="C35">
-        <v>38.25</v>
+        <v>91.46</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>434</v>
+        <v>210</v>
       </c>
       <c r="B36">
         <v>35</v>
       </c>
       <c r="C36">
-        <v>38.17</v>
+        <v>90.68</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>447</v>
+        <v>216</v>
       </c>
       <c r="B37">
         <v>36</v>
       </c>
       <c r="C37">
-        <v>38.090000000000003</v>
+        <v>90.5</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>460</v>
+        <v>222</v>
       </c>
       <c r="B38">
         <v>37</v>
       </c>
       <c r="C38">
-        <v>38.01</v>
+        <v>91.21</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>473</v>
+        <v>228</v>
       </c>
       <c r="B39">
         <v>38</v>
       </c>
       <c r="C39">
-        <v>37.92</v>
+        <v>90.73</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>486</v>
+        <v>234</v>
       </c>
       <c r="B40">
         <v>39</v>
       </c>
       <c r="C40">
-        <v>37.840000000000003</v>
+        <v>92.46</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>499</v>
+        <v>240</v>
       </c>
       <c r="B41">
         <v>40</v>
       </c>
       <c r="C41">
-        <v>37.75</v>
+        <v>91.48</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>512</v>
+        <v>246</v>
       </c>
       <c r="B42">
         <v>41</v>
       </c>
       <c r="C42">
-        <v>37.67</v>
+        <v>91.27</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>525</v>
+        <v>252</v>
       </c>
       <c r="B43">
         <v>42</v>
       </c>
       <c r="C43">
-        <v>37.590000000000003</v>
+        <v>92</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>538</v>
+        <v>258</v>
       </c>
       <c r="B44">
         <v>43</v>
       </c>
       <c r="C44">
-        <v>37.51</v>
+        <v>91.46</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>551</v>
+        <v>264</v>
       </c>
       <c r="B45">
         <v>44</v>
       </c>
       <c r="C45">
-        <v>37.43</v>
+        <v>90.25</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>564</v>
+        <v>270</v>
       </c>
       <c r="B46">
         <v>45</v>
       </c>
       <c r="C46">
-        <v>37.35</v>
+        <v>91.75</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>577</v>
+        <v>276</v>
       </c>
       <c r="B47">
         <v>46</v>
       </c>
       <c r="C47">
-        <v>37.26</v>
+        <v>91.94</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>590</v>
+        <v>282</v>
       </c>
       <c r="B48">
         <v>47</v>
       </c>
       <c r="C48">
-        <v>37.17</v>
+        <v>90.95</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>603</v>
+        <v>288</v>
       </c>
       <c r="B49">
         <v>48</v>
       </c>
       <c r="C49">
-        <v>37.08</v>
+        <v>58.72</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>616</v>
+        <v>294</v>
       </c>
       <c r="B50">
         <v>49</v>
       </c>
       <c r="C50">
-        <v>37.01</v>
+        <v>88.89</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>629</v>
+        <v>300</v>
       </c>
       <c r="B51">
         <v>50</v>
       </c>
       <c r="C51">
-        <v>36.93</v>
+        <v>91.25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added report, updated plots
</commit_message>
<xml_diff>
--- a/Plotting Results/EPA_CA2_X00129654.xlsx
+++ b/Plotting Results/EPA_CA2_X00129654.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{F8E4A1C6-9E75-42C3-9510-E8943789FFC0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{9BACC503-59B3-4831-9A13-6F8BB9E5BFA5}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -348,8 +348,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="E49" sqref="E49"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J23" sqref="J23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -367,552 +367,552 @@
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B2">
         <v>1</v>
       </c>
       <c r="C2">
-        <v>68.83</v>
+        <v>66.180000000000007</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>108</v>
+        <v>203</v>
       </c>
       <c r="B3">
         <v>2</v>
       </c>
       <c r="C3">
-        <v>68.73</v>
+        <v>66.12</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>118</v>
+        <v>298</v>
       </c>
       <c r="B4">
         <v>3</v>
       </c>
       <c r="C4">
-        <v>68.64</v>
+        <v>66.06</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>76</v>
+        <v>401</v>
       </c>
       <c r="B5">
         <v>4</v>
       </c>
       <c r="C5">
-        <v>68.55</v>
+        <v>66.010000000000005</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>91</v>
+        <v>502</v>
       </c>
       <c r="B6">
         <v>5</v>
       </c>
       <c r="C6">
-        <v>68.459999999999994</v>
+        <v>65.95</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>86</v>
+        <v>595</v>
       </c>
       <c r="B7">
         <v>6</v>
       </c>
       <c r="C7">
-        <v>68.37</v>
+        <v>65.89</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>101</v>
+        <v>698</v>
       </c>
       <c r="B8">
         <v>7</v>
       </c>
       <c r="C8">
-        <v>68.27</v>
+        <v>65.83</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>96</v>
+        <v>798</v>
       </c>
       <c r="B9">
         <v>8</v>
       </c>
       <c r="C9">
-        <v>68.180000000000007</v>
+        <v>65.78</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>70</v>
+        <v>891</v>
       </c>
       <c r="B10">
         <v>9</v>
       </c>
       <c r="C10">
-        <v>68.09</v>
+        <v>65.72</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>104</v>
+        <v>984</v>
       </c>
       <c r="B11">
         <v>10</v>
       </c>
       <c r="C11">
-        <v>68.010000000000005</v>
+        <v>65.66</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>85</v>
+        <v>1077</v>
       </c>
       <c r="B12">
         <v>11</v>
       </c>
       <c r="C12">
-        <v>67.92</v>
+        <v>65.599999999999994</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>93</v>
+        <v>1166</v>
       </c>
       <c r="B13">
         <v>12</v>
       </c>
       <c r="C13">
-        <v>67.83</v>
+        <v>65.55</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>110</v>
+        <v>1268</v>
       </c>
       <c r="B14">
         <v>13</v>
       </c>
       <c r="C14">
-        <v>67.739999999999995</v>
+        <v>65.489999999999995</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>101</v>
+        <v>1370</v>
       </c>
       <c r="B15">
         <v>14</v>
       </c>
       <c r="C15">
-        <v>67.650000000000006</v>
+        <v>65.430000000000007</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>92</v>
+        <v>1454</v>
       </c>
       <c r="B16">
         <v>15</v>
       </c>
       <c r="C16">
-        <v>67.56</v>
+        <v>65.37</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>112</v>
+        <v>1549</v>
       </c>
       <c r="B17">
         <v>16</v>
       </c>
       <c r="C17">
-        <v>67.48</v>
+        <v>65.319999999999993</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>102</v>
+        <v>1642</v>
       </c>
       <c r="B18">
         <v>17</v>
       </c>
       <c r="C18">
-        <v>67.39</v>
+        <v>65.260000000000005</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>93</v>
+        <v>1735</v>
       </c>
       <c r="B19">
         <v>18</v>
       </c>
       <c r="C19">
-        <v>67.3</v>
+        <v>65.2</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>98</v>
+        <v>1829</v>
       </c>
       <c r="B20">
         <v>19</v>
       </c>
       <c r="C20">
-        <v>67.22</v>
+        <v>65.150000000000006</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>86</v>
+        <v>1917</v>
       </c>
       <c r="B21">
         <v>20</v>
       </c>
       <c r="C21">
-        <v>67.13</v>
+        <v>65.09</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>85</v>
+        <v>2006</v>
       </c>
       <c r="B22">
         <v>21</v>
       </c>
       <c r="C22">
-        <v>67.040000000000006</v>
+        <v>65.03</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>92</v>
+        <v>2111</v>
       </c>
       <c r="B23">
         <v>22</v>
       </c>
       <c r="C23">
-        <v>66.959999999999994</v>
+        <v>64.98</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>92</v>
+        <v>2188</v>
       </c>
       <c r="B24">
         <v>23</v>
       </c>
       <c r="C24">
-        <v>66.87</v>
+        <v>64.92</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>87</v>
+        <v>2295</v>
       </c>
       <c r="B25">
         <v>24</v>
       </c>
       <c r="C25">
-        <v>66.78</v>
+        <v>64.87</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>87</v>
+        <v>2387</v>
       </c>
       <c r="B26">
         <v>25</v>
       </c>
       <c r="C26">
-        <v>66.7</v>
+        <v>64.81</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>102</v>
+        <v>2496</v>
       </c>
       <c r="B27">
         <v>26</v>
       </c>
       <c r="C27">
-        <v>66.61</v>
+        <v>64.760000000000005</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>97</v>
+        <v>2582</v>
       </c>
       <c r="B28">
         <v>27</v>
       </c>
       <c r="C28">
-        <v>66.53</v>
+        <v>64.7</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>108</v>
+        <v>2668</v>
       </c>
       <c r="B29">
         <v>28</v>
       </c>
       <c r="C29">
-        <v>66.45</v>
+        <v>64.650000000000006</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>76</v>
+        <v>2763</v>
       </c>
       <c r="B30">
         <v>29</v>
       </c>
       <c r="C30">
-        <v>66.36</v>
+        <v>64.59</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>77</v>
+        <v>2857</v>
       </c>
       <c r="B31">
         <v>30</v>
       </c>
       <c r="C31">
-        <v>66.28</v>
+        <v>64.540000000000006</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>63</v>
+        <v>2942</v>
       </c>
       <c r="B32">
         <v>31</v>
       </c>
       <c r="C32">
-        <v>66.19</v>
+        <v>64.48</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>88</v>
+        <v>3023</v>
       </c>
       <c r="B33">
         <v>32</v>
       </c>
       <c r="C33">
-        <v>66.11</v>
+        <v>64.430000000000007</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>109</v>
+        <v>3115</v>
       </c>
       <c r="B34">
         <v>33</v>
       </c>
       <c r="C34">
-        <v>66.02</v>
+        <v>64.37</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>82</v>
+        <v>3186</v>
       </c>
       <c r="B35">
         <v>34</v>
       </c>
       <c r="C35">
-        <v>65.94</v>
+        <v>64.319999999999993</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>86</v>
+        <v>3270</v>
       </c>
       <c r="B36">
         <v>35</v>
       </c>
       <c r="C36">
-        <v>65.849999999999994</v>
+        <v>64.260000000000005</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>95</v>
+        <v>3361</v>
       </c>
       <c r="B37">
         <v>36</v>
       </c>
       <c r="C37">
-        <v>65.77</v>
+        <v>64.209999999999994</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>70</v>
+        <v>3451</v>
       </c>
       <c r="B38">
         <v>37</v>
       </c>
       <c r="C38">
-        <v>65.69</v>
+        <v>64.150000000000006</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>84</v>
+        <v>3548</v>
       </c>
       <c r="B39">
         <v>38</v>
       </c>
       <c r="C39">
-        <v>65.599999999999994</v>
+        <v>64.099999999999994</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>75</v>
+        <v>3640</v>
       </c>
       <c r="B40">
         <v>39</v>
       </c>
       <c r="C40">
-        <v>65.52</v>
+        <v>64.040000000000006</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>93</v>
+        <v>3725</v>
       </c>
       <c r="B41">
         <v>40</v>
       </c>
       <c r="C41">
-        <v>65.44</v>
+        <v>63.99</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>111</v>
+        <v>3820</v>
       </c>
       <c r="B42">
         <v>41</v>
       </c>
       <c r="C42">
-        <v>65.36</v>
+        <v>63.93</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>93</v>
+        <v>3905</v>
       </c>
       <c r="B43">
         <v>42</v>
       </c>
       <c r="C43">
-        <v>65.28</v>
+        <v>63.88</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>93</v>
+        <v>3992</v>
       </c>
       <c r="B44">
         <v>43</v>
       </c>
       <c r="C44">
-        <v>65.2</v>
+        <v>63.83</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>71</v>
+        <v>4077</v>
       </c>
       <c r="B45">
         <v>44</v>
       </c>
       <c r="C45">
-        <v>65.12</v>
+        <v>63.77</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>85</v>
+        <v>4161</v>
       </c>
       <c r="B46">
         <v>45</v>
       </c>
       <c r="C46">
-        <v>65.040000000000006</v>
+        <v>63.72</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>91</v>
+        <v>4256</v>
       </c>
       <c r="B47">
         <v>46</v>
       </c>
       <c r="C47">
-        <v>64.95</v>
+        <v>63.66</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>94</v>
+        <v>4348</v>
       </c>
       <c r="B48">
         <v>47</v>
       </c>
       <c r="C48">
-        <v>64.87</v>
+        <v>63.61</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>101</v>
+        <v>4417</v>
       </c>
       <c r="B49">
         <v>48</v>
       </c>
       <c r="C49">
-        <v>64.790000000000006</v>
+        <v>63.56</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>93</v>
+        <v>4498</v>
       </c>
       <c r="B50">
         <v>49</v>
       </c>
       <c r="C50">
-        <v>64.72</v>
+        <v>63.5</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>106</v>
+        <v>4608</v>
       </c>
       <c r="B51">
         <v>50</v>
       </c>
       <c r="C51">
-        <v>64.64</v>
+        <v>63.45</v>
       </c>
     </row>
   </sheetData>

</xml_diff>